<commit_message>
fix: empty PTAs erroring out
</commit_message>
<xml_diff>
--- a/pta-template-6vwo.xlsx
+++ b/pta-template-6vwo.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27916"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86661AFB-3F1B-4BBC-8D0B-DE1827A152CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{34E71404-E8E3-41B5-8F53-B7A470CF4374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AK" sheetId="1" r:id="rId1"/>
+    <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -290,7 +290,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -366,6 +366,12 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -517,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -544,128 +550,134 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -928,7 +940,7 @@
   <dimension ref="A1:AO63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:G23"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -950,23 +962,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="36" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
       <c r="V1" s="1"/>
       <c r="W1" s="2" t="s">
         <v>1</v>
@@ -1037,25 +1049,25 @@
       </c>
     </row>
     <row r="2" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
       <c r="V2" s="1"/>
       <c r="W2" s="2" t="s">
         <v>1</v>
@@ -1096,25 +1108,25 @@
       <c r="AO2" s="3"/>
     </row>
     <row r="3" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="23" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
       <c r="V3" s="1"/>
       <c r="W3" s="2" t="s">
         <v>1</v>
@@ -1153,21 +1165,21 @@
       <c r="AO3" s="3"/>
     </row>
     <row r="4" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
       <c r="V4" s="1"/>
       <c r="W4" s="2" t="s">
         <v>1</v>
@@ -1206,31 +1218,31 @@
       <c r="AO4" s="3"/>
     </row>
     <row r="5" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="25" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20" t="s">
+      <c r="H5" s="12"/>
+      <c r="I5" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="27" t="s">
+      <c r="J5" s="36"/>
+      <c r="K5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
       <c r="V5" s="1"/>
       <c r="W5" s="2" t="s">
         <v>1</v>
@@ -1269,25 +1281,25 @@
       <c r="AO5" s="3"/>
     </row>
     <row r="6" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="26" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
       <c r="V6" s="1"/>
       <c r="W6" s="2" t="s">
         <v>1</v>
@@ -1323,25 +1335,25 @@
       <c r="AO6" s="3"/>
     </row>
     <row r="7" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="31" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
       <c r="V7" s="1"/>
       <c r="W7" s="2" t="s">
         <v>1</v>
@@ -1374,41 +1386,41 @@
       <c r="AO7" s="3"/>
     </row>
     <row r="8" spans="1:41" ht="129.75" customHeight="1">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="32" t="s">
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="32" t="s">
+      <c r="K8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="35" t="s">
+      <c r="M8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="21"/>
-      <c r="O8" s="32" t="s">
+      <c r="N8" s="47"/>
+      <c r="O8" s="22" t="s">
         <v>24</v>
       </c>
       <c r="V8" s="1"/>
@@ -1443,23 +1455,23 @@
       <c r="AO8" s="3"/>
     </row>
     <row r="9" spans="1:41" ht="24" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="35" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="21"/>
-      <c r="O9" s="19"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="12"/>
       <c r="V9" s="1"/>
       <c r="W9" s="2" t="s">
         <v>1</v>
@@ -1498,18 +1510,18 @@
       <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="11" t="s">
         <v>32</v>
       </c>
@@ -1522,10 +1534,10 @@
       <c r="L10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="M10" s="42" t="s">
+      <c r="M10" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="41"/>
+      <c r="N10" s="34"/>
       <c r="O10" s="11" t="s">
         <v>37</v>
       </c>
@@ -1561,21 +1573,21 @@
       <c r="AO10" s="3"/>
     </row>
     <row r="11" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="45"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="28"/>
       <c r="V11" s="1"/>
       <c r="W11" s="2" t="s">
         <v>38</v>
@@ -1602,21 +1614,21 @@
       <c r="AO11" s="1"/>
     </row>
     <row r="12" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="47"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="29"/>
       <c r="V12" s="1"/>
       <c r="W12" s="2" t="s">
         <v>38</v>
@@ -1643,21 +1655,21 @@
       <c r="AO12" s="1"/>
     </row>
     <row r="13" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
       <c r="V13" s="1"/>
       <c r="W13" s="2" t="s">
         <v>39</v>
@@ -1684,25 +1696,25 @@
       <c r="AO13" s="1"/>
     </row>
     <row r="14" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50" t="s">
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
       <c r="V14" s="1"/>
       <c r="W14" s="2" t="s">
         <v>39</v>
@@ -1713,29 +1725,29 @@
       <c r="Y14" s="1"/>
     </row>
     <row r="15" spans="1:41" ht="12.75">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="31" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
       <c r="V15" s="1"/>
       <c r="W15" s="2" t="s">
         <v>39</v>
@@ -1746,29 +1758,29 @@
       <c r="Y15" s="1"/>
     </row>
     <row r="16" spans="1:41" ht="25.5">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="51" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="51" t="s">
+      <c r="F16" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="51" t="s">
+      <c r="G16" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
       <c r="V16" s="1"/>
       <c r="W16" s="2" t="s">
         <v>39</v>
@@ -1779,23 +1791,23 @@
       <c r="Y16" s="1"/>
     </row>
     <row r="17" spans="1:25" ht="12.75">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
       <c r="V17" s="1"/>
       <c r="W17" s="2" t="s">
         <v>39</v>
@@ -1806,23 +1818,23 @@
       <c r="Y17" s="1"/>
     </row>
     <row r="18" spans="1:25" ht="12.75">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="49"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
       <c r="V18" s="1"/>
       <c r="W18" s="2" t="s">
         <v>39</v>
@@ -1833,113 +1845,113 @@
       <c r="Y18" s="1"/>
     </row>
     <row r="19" spans="1:25" ht="12.75">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="49"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
       <c r="V19" s="1"/>
       <c r="W19" s="2"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="1"/>
     </row>
     <row r="20" spans="1:25" ht="12.75">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="49"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
       <c r="V20" s="1"/>
       <c r="W20" s="2"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="1"/>
     </row>
     <row r="21" spans="1:25" ht="12.75">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="19"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
       <c r="V21" s="1"/>
       <c r="W21" s="2"/>
       <c r="X21" s="7"/>
       <c r="Y21" s="1"/>
     </row>
     <row r="22" spans="1:25" ht="12.75">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="19"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
       <c r="V22" s="1"/>
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="1:25" ht="12.75">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="19"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
       <c r="V23" s="1"/>
       <c r="Y23" s="1"/>
     </row>
@@ -2404,19 +2416,11 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:E5"/>
     <mergeCell ref="E11:H11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="I5:J5"/>
@@ -2428,11 +2432,19 @@
     <mergeCell ref="E9:H9"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="E10:H10"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" sqref="E16:E23" xr:uid="{00000000-0002-0000-0000-000003000000}">

</xml_diff>